<commit_message>
Verify ID locally. (WIP)
</commit_message>
<xml_diff>
--- a/KMS_batch_backend/bin/Debug/Input.xlsx
+++ b/KMS_batch_backend/bin/Debug/Input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>FullName</t>
   </si>
@@ -52,15 +52,27 @@
   </si>
   <si>
     <t>DZID</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>王德玉</t>
+  </si>
+  <si>
+    <t>37020319611025031X</t>
+  </si>
+  <si>
+    <t>黄俊龙</t>
+  </si>
+  <si>
+    <t>422822198807221014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,14 +115,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,16 +403,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -413,13 +428,13 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -433,10 +448,10 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="4">
@@ -450,14 +465,48 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="4">
         <v>30012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>327816381</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5">
+        <v>22579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>327816381</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5">
+        <v>22579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>